<commit_message>
updated template file v0.1
</commit_message>
<xml_diff>
--- a/source/template_entraid.xlsx
+++ b/source/template_entraid.xlsx
@@ -1,18 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28417"/>
-  <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{951B9E2E-1C48-40F5-88D8-5BB18FF5C195}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <workbookPr defaultThemeVersion="202300"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tecnimont-my.sharepoint.com/personal/t_ungetti_tecnimont_it/Documents/Documents/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{25D3C738-707F-4FF8-B365-29F1B1E79D7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="3" xr2:uid="{21921A5B-A43E-4691-A77C-2837A2BA3E96}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
     <sheet name="Groups" sheetId="2" r:id="rId2"/>
     <sheet name="Licenses" sheetId="3" r:id="rId3"/>
+    <sheet name="Resources" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,50 +38,10 @@
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Job Title</t>
-  </si>
-  <si>
-    <t>Mail</t>
-  </si>
-  <si>
-    <t>User Principal Name</t>
-  </si>
-  <si>
-    <t>OnPrem Domain Name</t>
-  </si>
-  <si>
-    <t>OnPrem Sync Enabled</t>
-  </si>
-  <si>
-    <t>Members</t>
-  </si>
-  <si>
-    <t>Placeholder</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -91,7 +57,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -99,58 +65,18 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -179,13 +105,13 @@
         <a:srgbClr val="E8E8E8"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="145F82"/>
+        <a:srgbClr val="156082"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="E87331"/>
+        <a:srgbClr val="E97132"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="186C24"/>
+        <a:srgbClr val="196B24"/>
       </a:accent3>
       <a:accent4>
         <a:srgbClr val="0F9ED5"/>
@@ -205,7 +131,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="020F0302020204030204"/>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -471,95 +397,56 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEE85009-B421-416C-BEF9-D625AA3CA2C8}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="5" max="5" width="18.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7A7347-490E-4906-8017-295813C8AA64}">
-  <dimension ref="A1:E1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E58C04B-1BD9-476C-9E0D-0F8E7C7D41B3}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60544C04-C9D5-41EE-8519-075E3E9EC7FE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D1D4D19-46A2-41A6-81F9-0D74B9B02911}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7734BF8F-F7D9-4515-A86E-4A7ED7E2499D}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>